<commit_message>
finish clean up and comments
</commit_message>
<xml_diff>
--- a/ProjectWorkingFolder/tickers.xlsx
+++ b/ProjectWorkingFolder/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Taahaa\projects\StockSystem\ProjectWorkingFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C8ADC-71A9-4382-BCC5-FD5DC5E00745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CFBF07-FEF1-4B68-AE2E-6E5282AC97E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed line by accident
</commit_message>
<xml_diff>
--- a/ProjectWorkingFolder/tickers.xlsx
+++ b/ProjectWorkingFolder/tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Taahaa\projects\StockSystem\ProjectWorkingFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CFBF07-FEF1-4B68-AE2E-6E5282AC97E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328F34A-91C2-448E-84B6-98C275AB7E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Rank</t>
   </si>
@@ -94,15 +94,6 @@
     <t>609.63</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>574.41</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -506,9 +497,6 @@
   </si>
   <si>
     <t>BERKSHIRE HATHAWAY</t>
-  </si>
-  <si>
-    <t>META PLATFORMS</t>
   </si>
   <si>
     <t>UNITEDHEALTH GROUP</t>
@@ -1008,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1038,7 +1026,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1052,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1066,7 +1054,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1080,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1094,7 +1082,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1108,7 +1096,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1122,7 +1110,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1136,7 +1124,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1150,7 +1138,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -1164,35 +1152,35 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -1206,7 +1194,7 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
@@ -1220,7 +1208,7 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
         <v>45</v>
@@ -1234,7 +1222,7 @@
         <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
@@ -1248,7 +1236,7 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -1262,7 +1250,7 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
         <v>54</v>
@@ -1276,7 +1264,7 @@
         <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -1290,7 +1278,7 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
         <v>60</v>
@@ -1304,7 +1292,7 @@
         <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>63</v>
@@ -1318,7 +1306,7 @@
         <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
         <v>66</v>
@@ -1332,7 +1320,7 @@
         <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
         <v>69</v>
@@ -1346,7 +1334,7 @@
         <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
@@ -1360,21 +1348,21 @@
         <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
         <v>79</v>
@@ -1388,7 +1376,7 @@
         <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
         <v>82</v>
@@ -1402,7 +1390,7 @@
         <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
         <v>85</v>
@@ -1416,7 +1404,7 @@
         <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
         <v>88</v>
@@ -1430,7 +1418,7 @@
         <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
         <v>91</v>
@@ -1444,7 +1432,7 @@
         <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
@@ -1458,7 +1446,7 @@
         <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C32" t="s">
         <v>97</v>
@@ -1472,21 +1460,21 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
         <v>104</v>
@@ -1500,7 +1488,7 @@
         <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
         <v>107</v>
@@ -1514,7 +1502,7 @@
         <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C36" t="s">
         <v>110</v>
@@ -1528,7 +1516,7 @@
         <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
         <v>113</v>
@@ -1542,21 +1530,21 @@
         <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>189</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="C39" t="s">
         <v>120</v>
@@ -1570,7 +1558,7 @@
         <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
         <v>123</v>
@@ -1584,7 +1572,7 @@
         <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C41" t="s">
         <v>126</v>
@@ -1598,7 +1586,7 @@
         <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C42" t="s">
         <v>129</v>
@@ -1612,7 +1600,7 @@
         <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C43" t="s">
         <v>132</v>
@@ -1626,7 +1614,7 @@
         <v>134</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
         <v>135</v>
@@ -1640,7 +1628,7 @@
         <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s">
         <v>138</v>
@@ -1654,7 +1642,7 @@
         <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
         <v>141</v>
@@ -1668,7 +1656,7 @@
         <v>143</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C47" t="s">
         <v>144</v>
@@ -1682,21 +1670,21 @@
         <v>146</v>
       </c>
       <c r="B48" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
         <v>151</v>
@@ -1710,33 +1698,19 @@
         <v>153</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C50" t="s">
         <v>154</v>
       </c>
       <c r="D50" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>156</v>
-      </c>
-      <c r="B51" t="s">
-        <v>199</v>
-      </c>
-      <c r="C51" t="s">
-        <v>157</v>
-      </c>
-      <c r="D51" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A4 A3 C3:E3 A6 A5 C5:E5 A8 A7 C7:E7 A10 A9 C9:E9 A12:E12 A11 C11:E11 A2 C2:E2 C4:E4 C6:E6 C10:E10 A15 A13 C13:E13 A14 C14:E14 A20 A16 C16:E16 A17 C17:E17 A18 C18:E18 A19 C19:E19 A26:E26 A21 C21:E21 C20:E20 A22 C22:E22 A23 C23:E23 A24 C24:E24 A25 C25:E25 A34:E34 A27 C27:E27 A28 C28:E28 A29 C29:E29 A30 C30:E30 A31 C31:E31 A32 C32:E32 A33 C33:E33 A49:E49 A35 C35:E35 A36 C36:E36 A37 C37:E37 A38 C38:E38 A39 C39:E39 A40 C40:E40 A41 C41:E41 A42 C42:E42 A43 C43:E43 A44 C44:E44 A45 C45:E45 A46 C46:E46 A47 C47:E47 A48 C48:E48 A52:E53 A50 C50:E50 A51 C51:E51 C15:E15 C8:E8 C1:E1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A4 A3 C3:E3 A6 A5 C5:E5 A8 A7 C7:E7 E9 E12 E11 A2 C2:E2 C4:E4 C6:E6 E10 E13 E14 E16 E17 E18 E19 E26 E21 E20 E22 E23 E24 E25 E34 E27 E28 E29 E30 E31 E32 E33 E49 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 A52:E53 E50 E51 E15 C8:E8 C1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>